<commit_message>
Completed with the Registration Process
</commit_message>
<xml_diff>
--- a/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dileep_K\Desktop\DCP_18\FrameworkPOM-master\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD57DC4-4E99-4F2D-B16C-E110A608880E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7B595A-FB8D-4B2B-9F96-38EFEAD95DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
   </bookViews>
@@ -204,16 +204,16 @@
     <t>ACCOUNT CREATED!</t>
   </si>
   <si>
-    <t xml:space="preserve"> Logged in as John Doe </t>
-  </si>
-  <si>
     <t>Account Deleted</t>
   </si>
   <si>
     <t>ACCOUNT DELETED!</t>
   </si>
   <si>
-    <t>op0eg80790093@ixunbo.com</t>
+    <t>Logged in as John Doe</t>
+  </si>
+  <si>
+    <t>kilhklikjop0eg8079093@ixunbo.com</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC914BC-115C-4E99-A655-A098063134BC}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="66" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="66" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -772,7 +772,7 @@
         <v>52</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
@@ -831,10 +831,10 @@
         <v>53</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added List of Products Test cases Contact Us Test cases
</commit_message>
<xml_diff>
--- a/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dileep_K\Desktop\DCP_18\FrameworkPOM-master\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABE4F3E-FB35-4D68-A411-D2ABDE9B7506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9054152E-3A72-4BEA-8034-386BC10E87EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="1290" windowWidth="14400" windowHeight="7270" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
   </bookViews>
   <sheets>
     <sheet name="regression" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
   <si>
     <t>TC101</t>
   </si>
@@ -244,6 +244,24 @@
   </si>
   <si>
     <t>Kanna18</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Just a sample check</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Typing the Message….</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>C:\Users\Dileep_K\Desktop</t>
   </si>
 </sst>
 </file>
@@ -626,7 +644,7 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="66" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="26" x14ac:dyDescent="0.35"/>
@@ -635,8 +653,8 @@
     <col min="2" max="2" width="57.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="35.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.1796875" style="3" bestFit="1" customWidth="1"/>
@@ -906,7 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -917,7 +935,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>66</v>
       </c>
@@ -927,8 +945,17 @@
       <c r="C19" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
@@ -937,6 +964,15 @@
       </c>
       <c r="C20" s="4" t="s">
         <v>60</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>